<commit_message>
file ipynb and excel update
</commit_message>
<xml_diff>
--- a/Proyecto_final_IN2023_update.xlsx
+++ b/Proyecto_final_IN2023_update.xlsx
@@ -5019,7 +5019,7 @@
         <v>500</v>
       </c>
       <c r="I73" t="n">
-        <v>424.1570541259982</v>
+        <v>500</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -27195,7 +27195,7 @@
         <v>200</v>
       </c>
       <c r="I425" t="n">
-        <v>424.1570541259982</v>
+        <v>800</v>
       </c>
       <c r="J425" t="inlineStr">
         <is>

</xml_diff>